<commit_message>
Formatted for sub 2
</commit_message>
<xml_diff>
--- a/SuppTables/Supp. Table 7 - HPO Genes discovered with accession subsets.xlsx
+++ b/SuppTables/Supp. Table 7 - HPO Genes discovered with accession subsets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\gdrive\umn\UMN\Documents\Manuscripts\ZmIonome Manuscript\WorkingDraft\SuppTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CamocoManuscript\SuppTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,36 +1145,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B19">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="25"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C19">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="25"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:G19">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>